<commit_message>
Add Sample Data for the New Database Columns
</commit_message>
<xml_diff>
--- a/Raw_Sample_Data_Tables.xlsx
+++ b/Raw_Sample_Data_Tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alma\Desktop\Portfolio Projects\C_Sharp\BudgetBuddy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3B4541A-EBA1-47BA-96B0-88E357B2B0C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE4CE351-A28F-447E-A9F3-ED092F6121A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{C51FD514-D897-4441-A03F-5E2DD9C24C4F}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{C51FD514-D897-4441-A03F-5E2DD9C24C4F}"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="111">
   <si>
     <t>Users</t>
   </si>
@@ -358,6 +358,15 @@
   </si>
   <si>
     <t>aaf71569-bfbc-4cb5-b6c1-1e29be7535f5</t>
+  </si>
+  <si>
+    <t>IsDefaultBudget</t>
+  </si>
+  <si>
+    <t>Threshhold</t>
+  </si>
+  <si>
+    <t>NULL</t>
   </si>
 </sst>
 </file>
@@ -448,7 +457,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -467,6 +476,7 @@
     <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1649,7 +1659,7 @@
   <dimension ref="A1:H117"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1749,6 +1759,12 @@
       <c r="C8" s="1" t="s">
         <v>44</v>
       </c>
+      <c r="D8" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -1760,6 +1776,12 @@
       <c r="C9">
         <v>1</v>
       </c>
+      <c r="D9" t="s">
+        <v>110</v>
+      </c>
+      <c r="E9" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -1771,6 +1793,12 @@
       <c r="C10">
         <v>2</v>
       </c>
+      <c r="D10" t="s">
+        <v>110</v>
+      </c>
+      <c r="E10" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -1781,6 +1809,12 @@
       </c>
       <c r="C11">
         <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>110</v>
+      </c>
+      <c r="E11" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1793,6 +1827,12 @@
       <c r="C12">
         <v>3</v>
       </c>
+      <c r="D12" t="s">
+        <v>110</v>
+      </c>
+      <c r="E12" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -1803,6 +1843,12 @@
       </c>
       <c r="C13">
         <v>2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>110</v>
+      </c>
+      <c r="E13" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -3552,9 +3598,10 @@
     <hyperlink ref="B19" r:id="rId6" xr:uid="{0228E848-6EA7-43D8-BA75-5B34C780A356}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
   <tableParts count="2">
-    <tablePart r:id="rId7"/>
     <tablePart r:id="rId8"/>
+    <tablePart r:id="rId9"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add Code to Get UsersBudgetNames by UserId
</commit_message>
<xml_diff>
--- a/Raw_Sample_Data_Tables.xlsx
+++ b/Raw_Sample_Data_Tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alma\Desktop\Portfolio Projects\C_Sharp\BudgetBuddy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE4CE351-A28F-447E-A9F3-ED092F6121A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CE6D6EB-0DE2-41D4-AAD4-74A946511D89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{C51FD514-D897-4441-A03F-5E2DD9C24C4F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="111">
   <si>
     <t>Users</t>
   </si>
@@ -457,7 +457,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -476,7 +476,6 @@
     <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1659,7 +1658,7 @@
   <dimension ref="A1:H117"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1759,10 +1758,10 @@
       <c r="C8" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="D8" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="E8" s="16" t="s">
+      <c r="E8" s="1" t="s">
         <v>109</v>
       </c>
     </row>
@@ -1776,8 +1775,8 @@
       <c r="C9">
         <v>1</v>
       </c>
-      <c r="D9" t="s">
-        <v>110</v>
+      <c r="D9">
+        <v>1</v>
       </c>
       <c r="E9" t="s">
         <v>110</v>

</xml_diff>

<commit_message>
Add Logic to Calculate Monthly Budget Overview
</commit_message>
<xml_diff>
--- a/Raw_Sample_Data_Tables.xlsx
+++ b/Raw_Sample_Data_Tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alma\Desktop\Portfolio Projects\C_Sharp\BudgetBuddy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CE6D6EB-0DE2-41D4-AAD4-74A946511D89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1347B9E-2ABC-4210-A05B-A06032332CA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{C51FD514-D897-4441-A03F-5E2DD9C24C4F}"/>
   </bookViews>
@@ -1657,8 +1657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3146CA4-E6F5-478D-B96D-BD19190C4163}">
   <dimension ref="A1:H117"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Display the Budget Overview Tables on the Home Page
</commit_message>
<xml_diff>
--- a/Raw_Sample_Data_Tables.xlsx
+++ b/Raw_Sample_Data_Tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alma\Desktop\Portfolio Projects\C_Sharp\BudgetBuddy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1347B9E-2ABC-4210-A05B-A06032332CA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C4AA8E0-F27D-44B9-A489-C86874FD85F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{C51FD514-D897-4441-A03F-5E2DD9C24C4F}"/>
   </bookViews>
@@ -1658,7 +1658,7 @@
   <dimension ref="A1:H117"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+      <selection activeCell="H52" sqref="H52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add Asyn to Database Operations
</commit_message>
<xml_diff>
--- a/Raw_Sample_Data_Tables.xlsx
+++ b/Raw_Sample_Data_Tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alma\Desktop\Portfolio Projects\C_Sharp\BudgetBuddy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C4AA8E0-F27D-44B9-A489-C86874FD85F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC02458C-FBE0-4685-816A-AD3E27890CE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{C51FD514-D897-4441-A03F-5E2DD9C24C4F}"/>
   </bookViews>
@@ -1657,8 +1657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3146CA4-E6F5-478D-B96D-BD19190C4163}">
   <dimension ref="A1:H117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="H52" sqref="H52"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="E55" sqref="E55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2428,7 +2428,7 @@
         <v>78</v>
       </c>
       <c r="E54">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F54">
         <v>0</v>

</xml_diff>

<commit_message>
Add Display Page for All Budget Items
</commit_message>
<xml_diff>
--- a/Raw_Sample_Data_Tables.xlsx
+++ b/Raw_Sample_Data_Tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alma\Desktop\Portfolio Projects\C_Sharp\BudgetBuddy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC02458C-FBE0-4685-816A-AD3E27890CE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5913F11-500D-4AA9-B676-66C22F056827}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{C51FD514-D897-4441-A03F-5E2DD9C24C4F}"/>
   </bookViews>
@@ -1657,8 +1657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3146CA4-E6F5-478D-B96D-BD19190C4163}">
   <dimension ref="A1:H117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="E55" sqref="E55"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>